<commit_message>
task status sheet updated
</commit_message>
<xml_diff>
--- a/Client-side/Client-side-flow.xlsx
+++ b/Client-side/Client-side-flow.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayushi\Desktop\ProjectEcommerceFSD\Client-side\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFBA35B-2CB5-42FC-A3FE-732E94D291CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +25,122 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+  <si>
+    <t>Modules</t>
+  </si>
+  <si>
+    <t>1)Home Module</t>
+  </si>
+  <si>
+    <t>Banner component</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Home component</t>
+  </si>
+  <si>
+    <t>header component</t>
+  </si>
+  <si>
+    <t>footer component</t>
+  </si>
+  <si>
+    <t>Customer_login component</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>Admin_login</t>
+  </si>
+  <si>
+    <t>App component</t>
+  </si>
+  <si>
+    <t>layout component</t>
+  </si>
+  <si>
+    <t>5)Admin module</t>
+  </si>
+  <si>
+    <t>4)auth module</t>
+  </si>
+  <si>
+    <t>3)Shared module</t>
+  </si>
+  <si>
+    <t>2)Product module</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>2)Services</t>
+  </si>
+  <si>
+    <t>1)Models :-</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>For customers</t>
+  </si>
+  <si>
+    <t>for products</t>
+  </si>
+  <si>
+    <t>For orders</t>
+  </si>
+  <si>
+    <t>Ayushi</t>
+  </si>
+  <si>
+    <t>Task Assigned To</t>
+  </si>
+  <si>
+    <t>Task Status</t>
+  </si>
+  <si>
+    <t>Mayank</t>
+  </si>
+  <si>
+    <t>on progress</t>
+  </si>
+  <si>
+    <t>Mayank and ayushi</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Mayank</t>
+  </si>
+  <si>
+    <t>6)Order module</t>
+  </si>
+  <si>
+    <t>7)App(main) module</t>
+  </si>
+  <si>
+    <t>8) Material Module</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +148,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +201,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +501,242 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2EC0F76-8C21-4FC6-9F5B-61EFDFB22242}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="27.90625" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="E13:E16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>